<commit_message>
seed 수정 && address 모델 추가
</commit_message>
<xml_diff>
--- a/xlsx/user.xlsx
+++ b/xlsx/user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="11775" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="20415" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="219">
   <si>
     <t>id</t>
   </si>
@@ -22,9 +22,15 @@
     <t>email</t>
   </si>
   <si>
+    <t>confirmation</t>
+  </si>
+  <si>
     <t>gomme9396@gmail.com</t>
   </si>
   <si>
+    <t>t</t>
+  </si>
+  <si>
     <t>rlsvkf1012@naver.com</t>
   </si>
   <si>
@@ -562,8 +568,109 @@
     <t>rkarbf13@naver.com</t>
   </si>
   <si>
-    <t>confirmation</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>huko1234@gmail.com</t>
+  </si>
+  <si>
+    <t>kimsungdo123@naver.com</t>
+  </si>
+  <si>
+    <t>wnsdud4406@naver.com</t>
+  </si>
+  <si>
+    <t>idea_hb@naver.com</t>
+  </si>
+  <si>
+    <t>sonyeun96@hanmail.net</t>
+  </si>
+  <si>
+    <t>dbstjq91@gmail.com</t>
+  </si>
+  <si>
+    <t>stdrive@naver.com</t>
+  </si>
+  <si>
+    <t>parkjc1111@naver.com</t>
+  </si>
+  <si>
+    <t>jae6120@naver.com</t>
+  </si>
+  <si>
+    <t>ktthee@naver.com</t>
+  </si>
+  <si>
+    <t>tkddlf323@hanmail.net</t>
+  </si>
+  <si>
+    <t>jg0428.lim@gmail.com</t>
+  </si>
+  <si>
+    <t>hjp9183@naver.com</t>
+  </si>
+  <si>
+    <t>yoona2222@hanmail.net</t>
+  </si>
+  <si>
+    <t>com6640131@naver.com</t>
+  </si>
+  <si>
+    <t>wns5167@naver.com</t>
+  </si>
+  <si>
+    <t>kevin4475@naver.com</t>
+  </si>
+  <si>
+    <t>thswndhkd22@naver.com</t>
+  </si>
+  <si>
+    <t>minho2230@naver.com</t>
+  </si>
+  <si>
+    <t>theking2983@gmail.com</t>
+  </si>
+  <si>
+    <t>cillic@hanmail.net</t>
+  </si>
+  <si>
+    <t>dear0724@naver.com</t>
+  </si>
+  <si>
+    <t>taengoole@naver.com</t>
+  </si>
+  <si>
+    <t>anminyoung77@gmail.com</t>
+  </si>
+  <si>
+    <t>mmjlee314@naver.com</t>
+  </si>
+  <si>
+    <t>2arm21c@naver.com</t>
+  </si>
+  <si>
+    <t>rkdrmsdka@naver.com</t>
+  </si>
+  <si>
+    <t>shiish@naver.com</t>
+  </si>
+  <si>
+    <t>kej4115@naver.com</t>
+  </si>
+  <si>
+    <t>kimmini10@naver.com</t>
+  </si>
+  <si>
+    <t>sb03147@naver.com</t>
+  </si>
+  <si>
+    <t>jun4250@naver.com</t>
+  </si>
+  <si>
+    <t>daeun0707@naver.com</t>
+  </si>
+  <si>
+    <t>jjunpopo@nate.com</t>
+  </si>
+  <si>
+    <t>gambler7712@naver.com</t>
   </si>
 </sst>
 </file>
@@ -1496,11 +1603,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
@@ -1512,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1520,10 +1625,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1531,10 +1636,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1542,10 +1647,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1553,10 +1658,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1564,10 +1669,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1575,10 +1680,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1586,10 +1691,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1597,10 +1702,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1608,10 +1713,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1619,10 +1724,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1630,10 +1735,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="b">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1641,10 +1746,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="b">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1652,10 +1757,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1663,10 +1768,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1674,10 +1779,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1685,10 +1790,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="b">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1696,10 +1801,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="b">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1707,10 +1812,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1718,10 +1823,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1729,10 +1834,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1740,10 +1845,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="b">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1751,10 +1856,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="b">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1762,10 +1867,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="b">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1773,10 +1878,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="b">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1784,10 +1889,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1795,10 +1900,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="b">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1806,10 +1911,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" t="b">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1817,10 +1922,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" t="b">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1828,10 +1933,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="b">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1839,10 +1944,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" t="b">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1850,10 +1955,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1861,10 +1966,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="b">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1872,10 +1977,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" t="b">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1883,10 +1988,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" t="b">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1894,10 +1999,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" t="b">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1905,10 +2010,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" t="b">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1916,10 +2021,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" t="b">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1927,10 +2032,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" t="b">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1938,10 +2043,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" t="b">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1949,10 +2054,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" t="b">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1960,10 +2065,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" t="b">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1971,10 +2076,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" t="b">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1982,10 +2087,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" t="b">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1993,10 +2098,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" t="b">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2004,10 +2109,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" t="b">
-        <v>1</v>
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2015,10 +2120,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" t="b">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2026,10 +2131,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" t="b">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2037,10 +2142,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" t="b">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2048,10 +2153,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" t="b">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2059,10 +2164,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" t="b">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2070,10 +2175,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" t="b">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2081,10 +2186,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" t="b">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2092,10 +2197,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" t="b">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2103,10 +2208,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" t="b">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2114,10 +2219,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" t="b">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2125,10 +2230,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" t="b">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2136,10 +2241,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" t="b">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2147,10 +2252,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" t="b">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2158,10 +2263,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" t="b">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2169,10 +2274,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" t="b">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2180,10 +2285,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" t="b">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2191,10 +2296,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2202,10 +2307,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" t="b">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2213,10 +2318,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" t="b">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2224,10 +2329,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" t="b">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2235,10 +2340,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" t="b">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2246,10 +2351,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" t="b">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2257,10 +2362,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" t="b">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2268,10 +2373,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" t="b">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2279,10 +2384,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
-      </c>
-      <c r="C71" t="b">
-        <v>1</v>
+        <v>73</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2290,10 +2395,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
-      </c>
-      <c r="C72" t="b">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2301,10 +2406,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>73</v>
-      </c>
-      <c r="C73" t="b">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2312,10 +2417,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" t="b">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2323,10 +2428,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" t="b">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2334,10 +2439,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
-      </c>
-      <c r="C76" t="b">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2345,10 +2450,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" t="b">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2356,10 +2461,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
-      </c>
-      <c r="C78" t="b">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2367,10 +2472,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
-      </c>
-      <c r="C79" t="b">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2378,10 +2483,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>80</v>
-      </c>
-      <c r="C80" t="b">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2389,10 +2494,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
-      </c>
-      <c r="C81" t="b">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2400,10 +2505,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
-      </c>
-      <c r="C82" t="b">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2411,10 +2516,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
-      </c>
-      <c r="C83" t="b">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2422,10 +2527,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
-      </c>
-      <c r="C84" t="b">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2433,10 +2538,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" t="b">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2444,10 +2549,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" t="b">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2455,10 +2560,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
-      </c>
-      <c r="C87" t="b">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2466,10 +2571,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
-      </c>
-      <c r="C88" t="b">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2477,10 +2582,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>89</v>
-      </c>
-      <c r="C89" t="b">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2488,10 +2593,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>90</v>
-      </c>
-      <c r="C90" t="b">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2499,10 +2604,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
-      </c>
-      <c r="C91" t="b">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2510,10 +2615,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>92</v>
-      </c>
-      <c r="C92" t="b">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2521,10 +2626,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>93</v>
-      </c>
-      <c r="C93" t="b">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="C93" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2532,10 +2637,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
-      </c>
-      <c r="C94" t="b">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2543,10 +2648,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>95</v>
-      </c>
-      <c r="C95" t="b">
-        <v>1</v>
+        <v>97</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2554,10 +2659,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>96</v>
-      </c>
-      <c r="C96" t="b">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2565,10 +2670,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
-      </c>
-      <c r="C97" t="b">
-        <v>1</v>
+        <v>99</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2576,10 +2681,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
-      </c>
-      <c r="C98" t="b">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2587,10 +2692,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
-      </c>
-      <c r="C99" t="b">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2598,10 +2703,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
-      </c>
-      <c r="C100" t="b">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2609,10 +2714,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
-      </c>
-      <c r="C101" t="b">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2620,10 +2725,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
-      </c>
-      <c r="C102" t="b">
-        <v>1</v>
+        <v>104</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -2631,10 +2736,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
-      </c>
-      <c r="C103" t="b">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2642,10 +2747,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>104</v>
-      </c>
-      <c r="C104" t="b">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -2653,10 +2758,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
-      </c>
-      <c r="C105" t="b">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2664,10 +2769,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
-      </c>
-      <c r="C106" t="b">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2675,10 +2780,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
-      </c>
-      <c r="C107" t="b">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2686,10 +2791,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
-      </c>
-      <c r="C108" t="b">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="C108" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2697,10 +2802,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
-      </c>
-      <c r="C109" t="b">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="C109" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2708,10 +2813,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
-      </c>
-      <c r="C110" t="b">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="C110" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2719,10 +2824,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
-      </c>
-      <c r="C111" t="b">
-        <v>1</v>
+        <v>113</v>
+      </c>
+      <c r="C111" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2730,10 +2835,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
-      </c>
-      <c r="C112" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2741,10 +2846,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
-      </c>
-      <c r="C113" t="b">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="C113" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2752,10 +2857,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
-      </c>
-      <c r="C114" t="b">
-        <v>1</v>
+        <v>116</v>
+      </c>
+      <c r="C114" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2763,10 +2868,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
-      </c>
-      <c r="C115" t="b">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="C115" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2774,10 +2879,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
-      </c>
-      <c r="C116" t="b">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="C116" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2785,10 +2890,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
-      </c>
-      <c r="C117" t="b">
-        <v>1</v>
+        <v>119</v>
+      </c>
+      <c r="C117" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2796,10 +2901,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
-      </c>
-      <c r="C118" t="b">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="C118" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2807,10 +2912,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
-      </c>
-      <c r="C119" t="b">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="C119" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2818,10 +2923,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
-      </c>
-      <c r="C120" t="b">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="C120" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2829,10 +2934,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
-      </c>
-      <c r="C121" t="b">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="C121" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2840,10 +2945,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
-      </c>
-      <c r="C122" t="b">
-        <v>1</v>
+        <v>124</v>
+      </c>
+      <c r="C122" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2851,10 +2956,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>123</v>
-      </c>
-      <c r="C123" t="b">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="C123" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2862,10 +2967,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
-      </c>
-      <c r="C124" t="b">
-        <v>1</v>
+        <v>126</v>
+      </c>
+      <c r="C124" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2873,10 +2978,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
-      </c>
-      <c r="C125" t="b">
-        <v>1</v>
+        <v>127</v>
+      </c>
+      <c r="C125" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2884,10 +2989,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>126</v>
-      </c>
-      <c r="C126" t="b">
-        <v>1</v>
+        <v>128</v>
+      </c>
+      <c r="C126" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2895,10 +3000,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>127</v>
-      </c>
-      <c r="C127" t="b">
-        <v>1</v>
+        <v>129</v>
+      </c>
+      <c r="C127" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2906,10 +3011,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
-      </c>
-      <c r="C128" t="b">
-        <v>1</v>
+        <v>130</v>
+      </c>
+      <c r="C128" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -2917,10 +3022,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>129</v>
-      </c>
-      <c r="C129" t="b">
-        <v>1</v>
+        <v>131</v>
+      </c>
+      <c r="C129" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -2928,10 +3033,10 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
-      </c>
-      <c r="C130" t="b">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="C130" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -2939,10 +3044,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
-      </c>
-      <c r="C131" t="b">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="C131" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -2950,10 +3055,10 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>132</v>
-      </c>
-      <c r="C132" t="b">
-        <v>1</v>
+        <v>134</v>
+      </c>
+      <c r="C132" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -2961,10 +3066,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>133</v>
-      </c>
-      <c r="C133" t="b">
-        <v>1</v>
+        <v>135</v>
+      </c>
+      <c r="C133" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -2972,10 +3077,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
-      </c>
-      <c r="C134" t="b">
-        <v>1</v>
+        <v>136</v>
+      </c>
+      <c r="C134" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -2983,10 +3088,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>135</v>
-      </c>
-      <c r="C135" t="b">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="C135" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -2994,10 +3099,10 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
-      </c>
-      <c r="C136" t="b">
-        <v>1</v>
+        <v>138</v>
+      </c>
+      <c r="C136" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -3005,10 +3110,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>137</v>
-      </c>
-      <c r="C137" t="b">
-        <v>1</v>
+        <v>139</v>
+      </c>
+      <c r="C137" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -3016,10 +3121,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
-      </c>
-      <c r="C138" t="b">
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="C138" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -3027,10 +3132,10 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>139</v>
-      </c>
-      <c r="C139" t="b">
-        <v>1</v>
+        <v>141</v>
+      </c>
+      <c r="C139" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -3038,10 +3143,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>140</v>
-      </c>
-      <c r="C140" t="b">
-        <v>1</v>
+        <v>142</v>
+      </c>
+      <c r="C140" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3049,10 +3154,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
-      </c>
-      <c r="C141" t="b">
-        <v>1</v>
+        <v>143</v>
+      </c>
+      <c r="C141" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -3060,10 +3165,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
-      </c>
-      <c r="C142" t="b">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="C142" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -3071,10 +3176,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>143</v>
-      </c>
-      <c r="C143" t="b">
-        <v>1</v>
+        <v>145</v>
+      </c>
+      <c r="C143" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -3082,10 +3187,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>144</v>
-      </c>
-      <c r="C144" t="b">
-        <v>1</v>
+        <v>146</v>
+      </c>
+      <c r="C144" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3093,10 +3198,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>145</v>
-      </c>
-      <c r="C145" t="b">
-        <v>1</v>
+        <v>147</v>
+      </c>
+      <c r="C145" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -3104,10 +3209,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>146</v>
-      </c>
-      <c r="C146" t="b">
-        <v>1</v>
+        <v>148</v>
+      </c>
+      <c r="C146" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -3115,10 +3220,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>147</v>
-      </c>
-      <c r="C147" t="b">
-        <v>1</v>
+        <v>149</v>
+      </c>
+      <c r="C147" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -3126,10 +3231,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>148</v>
-      </c>
-      <c r="C148" t="b">
-        <v>1</v>
+        <v>150</v>
+      </c>
+      <c r="C148" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -3137,10 +3242,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>149</v>
-      </c>
-      <c r="C149" t="b">
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="C149" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -3148,10 +3253,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>150</v>
-      </c>
-      <c r="C150" t="b">
-        <v>1</v>
+        <v>152</v>
+      </c>
+      <c r="C150" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -3159,10 +3264,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>151</v>
-      </c>
-      <c r="C151" t="b">
-        <v>1</v>
+        <v>153</v>
+      </c>
+      <c r="C151" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3170,10 +3275,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>152</v>
-      </c>
-      <c r="C152" t="b">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="C152" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -3181,10 +3286,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>153</v>
-      </c>
-      <c r="C153" t="b">
-        <v>1</v>
+        <v>155</v>
+      </c>
+      <c r="C153" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3192,10 +3297,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>154</v>
-      </c>
-      <c r="C154" t="b">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="C154" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -3203,10 +3308,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>155</v>
-      </c>
-      <c r="C155" t="b">
-        <v>1</v>
+        <v>157</v>
+      </c>
+      <c r="C155" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -3214,10 +3319,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>156</v>
-      </c>
-      <c r="C156" t="b">
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="C156" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3225,10 +3330,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>157</v>
-      </c>
-      <c r="C157" t="b">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="C157" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3236,10 +3341,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>158</v>
-      </c>
-      <c r="C158" t="b">
-        <v>1</v>
+        <v>160</v>
+      </c>
+      <c r="C158" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -3247,10 +3352,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
-      </c>
-      <c r="C159" t="b">
-        <v>1</v>
+        <v>161</v>
+      </c>
+      <c r="C159" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3258,10 +3363,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>160</v>
-      </c>
-      <c r="C160" t="b">
-        <v>1</v>
+        <v>162</v>
+      </c>
+      <c r="C160" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3269,10 +3374,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>161</v>
-      </c>
-      <c r="C161" t="b">
-        <v>1</v>
+        <v>163</v>
+      </c>
+      <c r="C161" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -3280,10 +3385,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>162</v>
-      </c>
-      <c r="C162" t="b">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="C162" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3291,10 +3396,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>163</v>
-      </c>
-      <c r="C163" t="b">
-        <v>1</v>
+        <v>165</v>
+      </c>
+      <c r="C163" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3302,10 +3407,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>164</v>
-      </c>
-      <c r="C164" t="b">
-        <v>1</v>
+        <v>166</v>
+      </c>
+      <c r="C164" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3313,10 +3418,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>165</v>
-      </c>
-      <c r="C165" t="b">
-        <v>1</v>
+        <v>167</v>
+      </c>
+      <c r="C165" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3324,10 +3429,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>166</v>
-      </c>
-      <c r="C166" t="b">
-        <v>1</v>
+        <v>168</v>
+      </c>
+      <c r="C166" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3335,10 +3440,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>167</v>
-      </c>
-      <c r="C167" t="b">
-        <v>1</v>
+        <v>169</v>
+      </c>
+      <c r="C167" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3346,10 +3451,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>168</v>
-      </c>
-      <c r="C168" t="b">
-        <v>1</v>
+        <v>170</v>
+      </c>
+      <c r="C168" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3357,10 +3462,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>169</v>
-      </c>
-      <c r="C169" t="b">
-        <v>1</v>
+        <v>171</v>
+      </c>
+      <c r="C169" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3368,10 +3473,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>170</v>
-      </c>
-      <c r="C170" t="b">
-        <v>1</v>
+        <v>172</v>
+      </c>
+      <c r="C170" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3379,10 +3484,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>171</v>
-      </c>
-      <c r="C171" t="b">
-        <v>1</v>
+        <v>173</v>
+      </c>
+      <c r="C171" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3390,10 +3495,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>172</v>
-      </c>
-      <c r="C172" t="b">
-        <v>1</v>
+        <v>174</v>
+      </c>
+      <c r="C172" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3401,10 +3506,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>173</v>
-      </c>
-      <c r="C173" t="b">
-        <v>1</v>
+        <v>175</v>
+      </c>
+      <c r="C173" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3412,10 +3517,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>174</v>
-      </c>
-      <c r="C174" t="b">
-        <v>1</v>
+        <v>176</v>
+      </c>
+      <c r="C174" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3423,10 +3528,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>175</v>
-      </c>
-      <c r="C175" t="b">
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="C175" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3434,10 +3539,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>176</v>
-      </c>
-      <c r="C176" t="b">
-        <v>1</v>
+        <v>178</v>
+      </c>
+      <c r="C176" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3445,10 +3550,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>177</v>
-      </c>
-      <c r="C177" t="b">
-        <v>1</v>
+        <v>179</v>
+      </c>
+      <c r="C177" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3456,10 +3561,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>178</v>
-      </c>
-      <c r="C178" t="b">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="C178" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3467,10 +3572,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>179</v>
-      </c>
-      <c r="C179" t="b">
-        <v>1</v>
+        <v>181</v>
+      </c>
+      <c r="C179" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3478,10 +3583,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>180</v>
-      </c>
-      <c r="C180" t="b">
-        <v>1</v>
+        <v>182</v>
+      </c>
+      <c r="C180" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3489,9 +3594,394 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
+        <v>183</v>
+      </c>
+      <c r="C181" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182">
         <v>181</v>
       </c>
-      <c r="C181" t="b">
+      <c r="B182" t="s">
+        <v>184</v>
+      </c>
+      <c r="C182" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" t="s">
+        <v>185</v>
+      </c>
+      <c r="C183" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
+        <v>186</v>
+      </c>
+      <c r="C184" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
+        <v>187</v>
+      </c>
+      <c r="C185" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" t="s">
+        <v>188</v>
+      </c>
+      <c r="C186" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
+        <v>189</v>
+      </c>
+      <c r="C187" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
+        <v>190</v>
+      </c>
+      <c r="C188" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" t="s">
+        <v>191</v>
+      </c>
+      <c r="C189" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" t="s">
+        <v>192</v>
+      </c>
+      <c r="C190" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" t="s">
+        <v>193</v>
+      </c>
+      <c r="C191" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" t="s">
+        <v>194</v>
+      </c>
+      <c r="C192" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" t="s">
+        <v>195</v>
+      </c>
+      <c r="C193" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" t="s">
+        <v>196</v>
+      </c>
+      <c r="C194" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
+        <v>197</v>
+      </c>
+      <c r="C195" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
+        <v>198</v>
+      </c>
+      <c r="C196" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
+        <v>199</v>
+      </c>
+      <c r="C197" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
+        <v>200</v>
+      </c>
+      <c r="C198" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
+        <v>201</v>
+      </c>
+      <c r="C199" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
+        <v>202</v>
+      </c>
+      <c r="C200" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
+        <v>203</v>
+      </c>
+      <c r="C201" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
+        <v>204</v>
+      </c>
+      <c r="C202" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
+        <v>205</v>
+      </c>
+      <c r="C203" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
+        <v>206</v>
+      </c>
+      <c r="C204" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" t="s">
+        <v>207</v>
+      </c>
+      <c r="C205" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
+        <v>208</v>
+      </c>
+      <c r="C206" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>209</v>
+      </c>
+      <c r="C207" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>210</v>
+      </c>
+      <c r="C208" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>211</v>
+      </c>
+      <c r="C209" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>212</v>
+      </c>
+      <c r="C210" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>213</v>
+      </c>
+      <c r="C211" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>214</v>
+      </c>
+      <c r="C212" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>215</v>
+      </c>
+      <c r="C213" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>216</v>
+      </c>
+      <c r="C214" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215" t="s">
+        <v>217</v>
+      </c>
+      <c r="C215" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" t="s">
+        <v>218</v>
+      </c>
+      <c r="C216" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>